<commit_message>
A number of data retreivel methods implemented, by use of the ELIA open data API.
</commit_message>
<xml_diff>
--- a/list_datapoints.xlsx
+++ b/list_datapoints.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="6708"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t>Data point</t>
   </si>
@@ -173,6 +173,27 @@
   </si>
   <si>
     <t>API ready</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>H-2 is closest available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is this? </t>
+  </si>
+  <si>
+    <t>H-2 is closest available in 15min resolution. However, there is one-minute imbalance price of H-1</t>
+  </si>
+  <si>
+    <t>ok, I think</t>
+  </si>
+  <si>
+    <t>available up to H-4</t>
+  </si>
+  <si>
+    <t>Not found</t>
   </si>
 </sst>
 </file>
@@ -541,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,6 +608,12 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -599,6 +626,12 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
@@ -611,6 +644,12 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -623,6 +662,12 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -635,6 +680,12 @@
       <c r="D6" t="s">
         <v>6</v>
       </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -648,6 +699,9 @@
       </c>
       <c r="D7" t="s">
         <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -661,6 +715,9 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
@@ -673,6 +730,9 @@
       <c r="D9" t="s">
         <v>16</v>
       </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -686,6 +746,12 @@
       </c>
       <c r="D10" t="s">
         <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -699,6 +765,12 @@
       <c r="D11" t="s">
         <v>6</v>
       </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
@@ -711,6 +783,12 @@
       <c r="D12" t="s">
         <v>6</v>
       </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -723,6 +801,12 @@
       <c r="D13" t="s">
         <v>6</v>
       </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
@@ -735,6 +819,12 @@
       <c r="D14" t="s">
         <v>6</v>
       </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
@@ -747,6 +837,12 @@
       <c r="D15" t="s">
         <v>6</v>
       </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
@@ -759,6 +855,12 @@
       <c r="D16" t="s">
         <v>6</v>
       </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -771,6 +873,12 @@
       <c r="D17" t="s">
         <v>6</v>
       </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -784,6 +892,9 @@
       </c>
       <c r="D18" t="s">
         <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -797,6 +908,9 @@
       <c r="D19" t="s">
         <v>16</v>
       </c>
+      <c r="F19" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -810,6 +924,9 @@
       </c>
       <c r="D20" t="s">
         <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -823,6 +940,9 @@
       <c r="D21" t="s">
         <v>16</v>
       </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
@@ -835,6 +955,9 @@
       <c r="D22" t="s">
         <v>16</v>
       </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
@@ -913,6 +1036,9 @@
       </c>
       <c r="D28" t="s">
         <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
       </c>
       <c r="F28" t="s">
         <v>44</v>

</xml_diff>